<commit_message>
Added Case Auto Entitlement Test cases
Added Case Auto Entitlement Test cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>fetchwo</t>
   </si>
@@ -65,12 +65,6 @@
     <t>FetchServiceContract</t>
   </si>
   <si>
-    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON RS_1022', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000kxZfw');insert service_contract;</t>
-  </si>
-  <si>
-    <t>Select Name , Id from SVMXC__Service_Contract__c where Name = 'SCON RS_1022' AND Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
     <t>SVMXC</t>
   </si>
   <si>
@@ -99,6 +93,19 @@
   </si>
   <si>
     <t>SVMXC__ServiceMax_Processes__c SP = new SVMXC__ServiceMax_Processes__c (SVMXC__IsStandard__c = true, SVMXC__ProcessID__c = 'PREV001_SamplePMProcess', Id = 'a18q00000004HOI');update SP;</t>
+  </si>
+  <si>
+    <t>CaseTriggerEnable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVMXC.COMM_Utils_ManageSettings cums = new SVMXC.COMM_Utils_ManageSettings(); 
+cums.SVMX_getInventoryProcessSteps('{"propertyKey": "SVMXC_CASE_Trigger1","status":"Enabled","orgId":"00Dq0000000933B"}'); </t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000kxZfw');insert service_contract;</t>
+  </si>
+  <si>
+    <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
   </si>
 </sst>
 </file>
@@ -157,8 +164,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,7 +238,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -245,6 +262,11 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -268,6 +290,11 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,10 +590,12 @@
     <col min="10" max="10" width="28.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="50.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="38.5" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="59.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -589,22 +618,25 @@
         <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -621,24 +653,27 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Changes to RS_10133.sah
Added Changes to RS_10133.sah
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -32,12 +32,6 @@
     <t>fetchwo</t>
   </si>
   <si>
-    <t>Select Name , Id from SVMXC__Service_Order__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
-    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
-  </si>
-  <si>
     <t>CreateWorkOrderOpen</t>
   </si>
   <si>
@@ -106,6 +100,12 @@
   </si>
   <si>
     <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
+  </si>
+  <si>
+    <t>Select Name , Id,FORMAT(SVMXC__Actual_Initial_Response__c), FORMAT(SVMXC__Actual_Onsite_Response__c) from SVMXC__Service_Order__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
   </si>
 </sst>
 </file>
@@ -164,8 +164,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,7 +242,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -267,6 +271,8 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -295,6 +301,8 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,84 +605,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding RS_10131.sah to the test-cases
Adding RS_10131.sah to the test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -164,8 +164,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -242,7 +244,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +275,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -303,6 +306,7 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,6 +689,9 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Made changes to the user
Made changes to the user
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>fetchaccount</t>
   </si>
   <si>
-    <t>Select Name , Id from Account where Name = 'Account Automation 1' AND Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
     <t>CreateServiceContract</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>005q0000003GGfP</t>
   </si>
   <si>
     <t>OrgDetails</t>
@@ -100,15 +94,9 @@
     <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000kxZfw');insert service_contract;</t>
   </si>
   <si>
-    <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
     <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
   </si>
   <si>
-    <t>Select Name , Id,FORMAT(SVMXC__Actual_Initial_Response__c), FORMAT(SVMXC__Actual_Onsite_Response__c) from SVMXC__Service_Order__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
     <t>SVMXDEV__Service_Order__c WO = new SVMXDEV__Service_Order__c ( SVMXDEV__Company__c = '0010x00000BzwYI', SVMXDEV__Order_Status__c = 'Canceled' ,SVMXDEV__Country__c = 'United States', SVMXDEV__Sub_Status__c = 'Resolved', SVMXDEV__Priority__c = 'High');insert WO;</t>
   </si>
   <si>
@@ -134,6 +122,18 @@
   </si>
   <si>
     <t>Select Name ,Id,FORMAT(SVMXDEV__Actual_Initial_Response__c), FORMAT(SVMXDEV__Actual_Onsite_Response__c) from SVMXDEV__Service_Order__c where Createdby.Id = '0050x000000QaEC' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>Select Name , Id,FORMAT(SVMXC__Actual_Initial_Response__c), FORMAT(SVMXC__Actual_Onsite_Response__c) from SVMXC__Service_Order__c where Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>Select Name , Id from Account where Name = 'Account Automation 1' AND Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>0051I000000guzk</t>
   </si>
 </sst>
 </file>
@@ -192,8 +192,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -278,7 +280,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -313,6 +315,7 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -347,6 +350,7 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -624,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,36 +668,36 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -702,31 +706,31 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -742,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -777,51 +781,51 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding changes to BORegression test-cases
Adding changes to BORegression test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -36,9 +36,6 @@
     <t>CreateWorkOrderOpen</t>
   </si>
   <si>
-    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Canceled' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
-  </si>
-  <si>
     <t>CreateWorkOrderCanceled</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>001q000000kxZfw</t>
   </si>
   <si>
     <t>Username</t>
@@ -91,12 +85,6 @@
 cums.SVMX_getInventoryProcessSteps('{"propertyKey": "SVMXC_CASE_Trigger1","status":"Enabled","orgId":"00Dq0000000933B"}'); </t>
   </si>
   <si>
-    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000kxZfw');insert service_contract;</t>
-  </si>
-  <si>
-    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000kxZfw', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
-  </si>
-  <si>
     <t>SVMXDEV__Service_Order__c WO = new SVMXDEV__Service_Order__c ( SVMXDEV__Company__c = '0010x00000BzwYI', SVMXDEV__Order_Status__c = 'Canceled' ,SVMXDEV__Country__c = 'United States', SVMXDEV__Sub_Status__c = 'Resolved', SVMXDEV__Priority__c = 'High');insert WO;</t>
   </si>
   <si>
@@ -134,6 +122,18 @@
   </si>
   <si>
     <t>0051I000000guzk</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '0010x00000CIjok', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '0010x00000CIjok', SVMXC__Order_Status__c = 'Canceled' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '0010x00000CIjok');insert service_contract;</t>
+  </si>
+  <si>
+    <t>0010x00000CIjok</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,78 +659,78 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -772,60 +772,60 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the BackOffice Sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
+++ b/svmx/test_lab/test_cases/backOffice/bo_excleData/BORegressionDatasheet.xlsx
@@ -112,28 +112,28 @@
     <t>Select Name ,Id,FORMAT(SVMXDEV__Actual_Initial_Response__c), FORMAT(SVMXDEV__Actual_Onsite_Response__c) from SVMXDEV__Service_Order__c where Createdby.Id = '0050x000000QaEC' Order by CreatedDate DESC Limit 1</t>
   </si>
   <si>
-    <t>Select Name , Id,FORMAT(SVMXC__Actual_Initial_Response__c), FORMAT(SVMXC__Actual_Onsite_Response__c) from SVMXC__Service_Order__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
-    <t>Select Name , Id from Account where Name = 'Account Automation 1' AND Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
-    <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '005q0000003GGfP' Order by CreatedDate DESC Limit 1</t>
-  </si>
-  <si>
-    <t>005q0000003GGfP</t>
-  </si>
-  <si>
-    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000irAHS', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
-  </si>
-  <si>
-    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '001q000000irAHS', SVMXC__Order_Status__c = 'Canceled' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
-  </si>
-  <si>
-    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '001q000000irAHS');insert service_contract;</t>
-  </si>
-  <si>
-    <t>001q000000irAHS</t>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '0010x000004TMut', SVMXC__Order_Status__c = 'Open' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High',SVMXC__Actual_Initial_Response__c = System.Today(),SVMXC__Actual_Onsite_Response__c = System.Today() - 1 );insert WO;</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Order__c WO = new SVMXC__Service_Order__c ( SVMXC__Company__c = '0010x000004TMut', SVMXC__Order_Status__c = 'Canceled' ,SVMXC__Country__c = 'United States', SVMXC__Sub_Status__c = 'Resolved', SVMXC__Priority__c = 'High');insert WO;</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Contract__c service_contract = New SVMXC__Service_Contract__c (Name = 'SCON BO Regression', SVMXC__Active__c = true , SVMXC__All_Contacts_Covered__c = true , SVMXC__Company__c = '0010x000004TMut');insert service_contract;</t>
+  </si>
+  <si>
+    <t>0010x000004TMut</t>
+  </si>
+  <si>
+    <t>Select Name , Id,FORMAT(SVMXC__Actual_Initial_Response__c), FORMAT(SVMXC__Actual_Onsite_Response__c) from SVMXC__Service_Order__c where Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>Select Name , Id from Account where Name = 'Account Automation 1' AND Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>Select Name , Id from SVMXC__Service_Contract__c where Createdby.Id = '0051I000000guzk' Order by CreatedDate DESC Limit 1</t>
+  </si>
+  <si>
+    <t>0051I000000guzk</t>
   </si>
 </sst>
 </file>
@@ -192,8 +192,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -280,7 +282,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +318,7 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -351,6 +354,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,34 +698,34 @@
     </row>
     <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>

</xml_diff>